<commit_message>
tabla expedientes y provincias
</commit_message>
<xml_diff>
--- a/documentacion/tablas.xlsx
+++ b/documentacion/tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Herd\ggrc_gestion\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F760E521-079B-462E-AEE8-2F0E0F944C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEF2E27-F7B6-4570-8AC8-AC33F65F9AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86AA3994-8391-48BC-ACCC-EF9042BB5443}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>fecha_tdrs_elevacion</t>
   </si>
   <si>
-    <t>gde_firma_dieccion_tdrs</t>
-  </si>
-  <si>
     <t>monto_solicitud</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>fecha_apobacion_if</t>
   </si>
   <si>
-    <t>gde_informe_final</t>
-  </si>
-  <si>
     <t>fecha_envio_biblioteca</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>localidad</t>
+  </si>
+  <si>
+    <t>gde_tdrs_firma_dieccion</t>
+  </si>
+  <si>
+    <t>gde_aprobacion_if</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,13 +537,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -565,21 +565,21 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -614,122 +614,122 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>